<commit_message>
Changed phase offset to pi/2. Similar BER to Div&Sim.
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NASA Project Files\dpsk Non-Coher N=2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/NASA-Simulink-Projects/Simulink Upload/dpsk Non-Coher N=2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{24770109-0FD4-4013-893C-4C7091224781}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
+    <workbookView xWindow="3012" yWindow="1044" windowWidth="17280" windowHeight="8964" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1115,16 +1115,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>446942</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>71804</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>452804</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>118696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>153865</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>148004</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>159727</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>13189</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1449,15 +1449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5131BDC8-1059-4AC7-A3F1-9BCFD93C04A4}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>7</f>
         <v>7</v>
@@ -1486,8 +1486,12 @@
         <f>3*10^-3</f>
         <v>3.0000000000000001E-3</v>
       </c>
+      <c r="D3">
+        <f>0.0034</f>
+        <v>3.3999999999999998E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>8</f>
         <v>8</v>
@@ -1500,8 +1504,12 @@
         <f>10^-3</f>
         <v>1E-3</v>
       </c>
+      <c r="D4">
+        <f>0.0009999</f>
+        <v>9.9989999999999996E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>9</f>
         <v>9</v>
@@ -1514,8 +1522,12 @@
         <f>2*10^-4</f>
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="D5">
+        <f>0.00019</f>
+        <v>1.9000000000000001E-4</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>10</f>
         <v>10</v>
@@ -1528,8 +1540,12 @@
         <f>3*10^-5</f>
         <v>3.0000000000000004E-5</v>
       </c>
+      <c r="D6">
+        <f>0.00001</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>11</f>
         <v>11</v>
@@ -1539,7 +1555,7 @@
         <v>4.4600000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>12</f>
         <v>12</v>
@@ -1549,7 +1565,7 @@
         <v>3.1399999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>13</f>
         <v>13</v>

</xml_diff>

<commit_message>
Corrected M-ary DPSK Code with Non-Coherent Detection N=2
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/NASA-Simulink-Projects/Simulink Upload/dpsk Non-Coher N=2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{24770109-0FD4-4013-893C-4C7091224781}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{382F0336-4B34-4220-9083-F81FA1576740}"/>
   <bookViews>
-    <workbookView xWindow="3012" yWindow="1044" windowWidth="17280" windowHeight="8964" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,18 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>SNR</t>
-  </si>
-  <si>
-    <t>BER</t>
   </si>
   <si>
     <t>DBPSK</t>
   </si>
   <si>
     <t>Binary</t>
+  </si>
+  <si>
+    <t>Div&amp;Sim</t>
+  </si>
+  <si>
+    <t>My Model</t>
   </si>
 </sst>
 </file>
@@ -114,6 +117,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Non</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>-Coherent Detection M=2, N=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -158,7 +190,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BER</c:v>
+                  <c:v>Div&amp;Sim</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -203,15 +235,6 @@
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -222,25 +245,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9.9989999999999996E-2</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7389999999999995E-2</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.2190000000000004E-2</c:v>
+                  <c:v>2.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8090000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.4600000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1399999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2800000000000001E-2</c:v>
+                  <c:v>3.0000000000000004E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,6 +274,9 @@
               <c:f>Sheet1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Model</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -303,15 +320,6 @@
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -322,16 +330,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>3.3999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>9.9989999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0000000000000001E-4</c:v>
+                  <c:v>1.9000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000004E-5</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1115,16 +1123,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>452804</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>118696</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>470389</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>130418</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>159727</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>13189</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>177312</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>24911</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1449,130 +1457,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5131BDC8-1059-4AC7-A3F1-9BCFD93C04A4}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>7</f>
         <v>7</v>
       </c>
       <c r="B3">
-        <f>0.09999</f>
-        <v>9.9989999999999996E-2</v>
-      </c>
-      <c r="C3">
         <f>3*10^-3</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <f>0.0034</f>
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>8</f>
         <v>8</v>
       </c>
       <c r="B4">
-        <f>0.08739</f>
-        <v>8.7389999999999995E-2</v>
-      </c>
-      <c r="C4">
         <f>10^-3</f>
         <v>1E-3</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <f>0.0009999</f>
         <v>9.9989999999999996E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>9</f>
         <v>9</v>
       </c>
       <c r="B5">
-        <f>0.07219</f>
-        <v>7.2190000000000004E-2</v>
-      </c>
-      <c r="C5">
         <f>2*10^-4</f>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <f>0.00019</f>
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="B6">
-        <f>0.05809</f>
-        <v>5.8090000000000003E-2</v>
-      </c>
-      <c r="C6">
         <f>3*10^-5</f>
         <v>3.0000000000000004E-5</v>
       </c>
-      <c r="D6">
-        <f>0.00001</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f>11</f>
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <f>0.0446</f>
-        <v>4.4600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f>12</f>
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <f>0.0314</f>
-        <v>3.1399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f>13</f>
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <f>0.0228</f>
-        <v>2.2800000000000001E-2</v>
+      <c r="C6">
+        <f>0.00004</f>
+        <v>4.0000000000000003E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel File to Reflect Findings
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/NASA-Simulink-Projects/Simulink Upload/dpsk Non-Coher N=2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{382F0336-4B34-4220-9083-F81FA1576740}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AA655603-8770-42C5-87EC-4DFDD8DE723A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>SNR</t>
   </si>
@@ -41,13 +41,16 @@
     <t>DBPSK</t>
   </si>
   <si>
-    <t>Binary</t>
-  </si>
-  <si>
     <t>Div&amp;Sim</t>
   </si>
   <si>
     <t>My Model</t>
+  </si>
+  <si>
+    <t>DQPSK</t>
+  </si>
+  <si>
+    <t>8-PSK</t>
   </si>
 </sst>
 </file>
@@ -146,6 +149,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21667779662950834"/>
+          <c:y val="2.9082770633882267E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -154,26 +165,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -182,8 +173,144 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Div&amp;Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0000000000000004E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D026-4A38-BD5B-EBD3589CCDF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.3999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9989999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000003E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D026-4A38-BD5B-EBD3589CCDF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$2</c:f>
@@ -262,13 +389,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B84-4A09-B735-EF132D5D7578}"/>
+              <c16:uniqueId val="{00000002-D026-4A38-BD5B-EBD3589CCDF0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$2</c:f>
@@ -347,7 +474,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0B84-4A09-B735-EF132D5D7578}"/>
+              <c16:uniqueId val="{00000004-D026-4A38-BD5B-EBD3589CCDF0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -487,6 +614,473 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Non-Coherent Detection M=4, N=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40393744531933506"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Div&amp;Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9999999999999996E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B0C-4888-8FC9-CBC27F53C437}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6830000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7099999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8999999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0000000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4B0C-4888-8FC9-CBC27F53C437}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1382462351"/>
+        <c:axId val="1382462767"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1382462351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1382462767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1382462767"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1382462351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -528,6 +1122,501 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Non-Coherent Detection M=8, N=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Div&amp;Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9999999999999996E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19D9-4091-88A2-F0C4D6AE0CE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>My Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6990000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4700000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8900000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-19D9-4091-88A2-F0C4D6AE0CE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1236733503"/>
+        <c:axId val="1236741407"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1236733503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1236741407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1236741407"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1236733503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -603,6 +1692,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1119,20 +2248,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>470389</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>130418</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>98355</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>177312</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>24911</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>107661</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1152,6 +2797,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>164122</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>128953</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4F6B8B0-C83D-45D2-9BB1-2E476B9DA3F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>497541</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>8963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>466164</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>62750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85772E85-B667-41F8-8E65-0435EC354A76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1457,34 +3174,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5131BDC8-1059-4AC7-A3F1-9BCFD93C04A4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M24:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>7</f>
         <v>7</v>
@@ -1497,8 +3235,32 @@
         <f>0.0034</f>
         <v>3.3999999999999998E-3</v>
       </c>
+      <c r="J3">
+        <f>7</f>
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <f>10^-2</f>
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <f>0.01683</f>
+        <v>1.6830000000000001E-2</v>
+      </c>
+      <c r="P3">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="Q3">
+        <f>0.008</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="R3">
+        <f>0.01699</f>
+        <v>1.6990000000000002E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>8</f>
         <v>8</v>
@@ -1511,8 +3273,32 @@
         <f>0.0009999</f>
         <v>9.9989999999999996E-4</v>
       </c>
+      <c r="J4">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <f>0.008</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L4">
+        <f>0.00771</f>
+        <v>7.7099999999999998E-3</v>
+      </c>
+      <c r="P4">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="Q4">
+        <f>0.0045</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="R4">
+        <f>0.00747</f>
+        <v>7.4700000000000001E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>9</f>
         <v>9</v>
@@ -1525,8 +3311,32 @@
         <f>0.00019</f>
         <v>1.9000000000000001E-4</v>
       </c>
+      <c r="J5">
+        <f>9</f>
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <f>0.002</f>
+        <v>2E-3</v>
+      </c>
+      <c r="L5">
+        <f>0.0029</f>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="P5">
+        <f>13</f>
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <f>0.001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="R5">
+        <f>0.00289</f>
+        <v>2.8900000000000002E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>10</f>
         <v>10</v>
@@ -1538,6 +3348,82 @@
       <c r="C6">
         <f>0.00004</f>
         <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="J6">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <f>0.0005</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L6">
+        <f>0.00089</f>
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="P6">
+        <f>14</f>
+        <v>14</v>
+      </c>
+      <c r="Q6">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="R6">
+        <f>0.00058</f>
+        <v>5.8E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f>11</f>
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <f>0.0001</f>
+        <v>1E-4</v>
+      </c>
+      <c r="L7">
+        <f>0.00009</f>
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="P7">
+        <f>15</f>
+        <v>15</v>
+      </c>
+      <c r="Q7">
+        <f>0.00008</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="R7">
+        <f>0.00021</f>
+        <v>2.1000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <f>0.000008</f>
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="L8">
+        <f>0.00002</f>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="P8">
+        <f>16</f>
+        <v>16</v>
+      </c>
+      <c r="Q8">
+        <f>0.000008</f>
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="R8">
+        <f>0.00003</f>
+        <v>3.0000000000000001E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a modulo step to each of the 3 branches after the constellation subtraction step. This was a major improvement to the model's sensitivity to AWGN. The BER is still slightly off from Div&Sim, but it is very close. The excel file has been updated to show these improvements.
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/NASA-Simulink-Projects/Simulink Upload/dpsk Non-Coher N=2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/Simulink Holding Folder/Simulink Upload/dpsk Non-Coher N=2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AA655603-8770-42C5-87EC-4DFDD8DE723A}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C30A33E1-7780-4347-A68A-DAF936191834}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
+    <workbookView xWindow="3360" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>SNR</t>
   </si>
@@ -44,13 +44,16 @@
     <t>Div&amp;Sim</t>
   </si>
   <si>
-    <t>My Model</t>
-  </si>
-  <si>
     <t>DQPSK</t>
   </si>
   <si>
     <t>8-PSK</t>
+  </si>
+  <si>
+    <t>P. N=3</t>
+  </si>
+  <si>
+    <t>P. N=2</t>
   </si>
 </sst>
 </file>
@@ -86,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,7 +148,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>-Coherent Detection M=2, N=2</a:t>
+              <a:t>-Coherent Detection M=2, N=2,3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -153,8 +157,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.21667779662950834"/>
-          <c:y val="2.9082770633882267E-2"/>
+          <c:x val="0.21026800957034639"/>
+          <c:y val="3.231723172266291E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -173,18 +177,10 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Div&amp;Sim</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Div&amp;Simon</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -193,10 +189,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -214,10 +210,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
@@ -236,91 +232,15 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D026-4A38-BD5B-EBD3589CCDF0}"/>
+              <c16:uniqueId val="{00000003-7E8F-48B7-BFAC-365A656D806F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>My Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.3999999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.9989999999999996E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000003E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D026-4A38-BD5B-EBD3589CCDF0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Div&amp;Sim</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>P. N=2</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -332,24 +252,13 @@
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -367,21 +276,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>3.3999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>9.9989999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0000000000000001E-4</c:v>
+                  <c:v>1.9000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000004E-5</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,52 +298,27 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D026-4A38-BD5B-EBD3589CCDF0}"/>
+              <c16:uniqueId val="{00000004-7E8F-48B7-BFAC-365A656D806F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>My Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>P. N=3</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="19050">
               <a:noFill/>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -452,21 +336,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>Sheet1!$D$3:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3999999999999998E-3</c:v>
+                  <c:v>3.0699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9989999999999996E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000003E-5</c:v>
+                  <c:v>8.8000000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00E+00">
+                  <c:v>1.6000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00E+00">
+                  <c:v>1.7E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -474,7 +358,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D026-4A38-BD5B-EBD3589CCDF0}"/>
+              <c16:uniqueId val="{00000005-7E8F-48B7-BFAC-365A656D806F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -703,7 +587,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Non-Coherent Detection M=4, N=2</a:t>
+              <a:t>Non-Coherent Detection M=4, N=2,3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -712,8 +596,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.40393744531933506"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.29465663825770139"/>
+          <c:y val="2.570352749802177E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -857,7 +741,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>My Model</c:v>
+                  <c:v>P. N=2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -942,6 +826,95 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4B0C-4888-8FC9-CBC27F53C437}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>N=3 Peyton</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.379E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7600000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9599999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>7.6000000000000004E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C726-456D-BEB3-779DA3EC35CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1199,7 +1172,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Non-Coherent Detection M=8, N=2</a:t>
+              <a:t>Non-Coherent Detection M=8, N=2,3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1345,7 +1318,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>My Model</c:v>
+                  <c:v>P. N=2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1430,6 +1403,95 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-19D9-4091-88A2-F0C4D6AE0CE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>P. N=3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$3:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2319999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6179999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3420000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.92E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9999999999999996E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6B6B-47B6-802C-BB6C0346E860}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2769,15 +2831,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>98355</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>107661</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>511245</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2804,16 +2866,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>562538</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>164122</xdr:rowOff>
+      <xdr:rowOff>17929</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>128953</xdr:rowOff>
+      <xdr:colOff>502023</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>44822</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2841,15 +2903,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>497541</xdr:colOff>
+      <xdr:colOff>497542</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>8963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>466164</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>62750</xdr:rowOff>
+      <xdr:colOff>555812</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>98612</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3174,26 +3236,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5131BDC8-1059-4AC7-A3F1-9BCFD93C04A4}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M24:M25"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3201,7 +3263,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
@@ -3210,7 +3275,10 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
       </c>
       <c r="P2" t="s">
         <v>0</v>
@@ -3219,10 +3287,13 @@
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>7</f>
         <v>7</v>
@@ -3235,6 +3306,10 @@
         <f>0.0034</f>
         <v>3.3999999999999998E-3</v>
       </c>
+      <c r="D3">
+        <f>0.00307</f>
+        <v>3.0699999999999998E-3</v>
+      </c>
       <c r="J3">
         <f>7</f>
         <v>7</v>
@@ -3247,6 +3322,10 @@
         <f>0.01683</f>
         <v>1.6830000000000001E-2</v>
       </c>
+      <c r="M3">
+        <f>0.01379</f>
+        <v>1.379E-2</v>
+      </c>
       <c r="P3">
         <f>11</f>
         <v>11</v>
@@ -3259,8 +3338,12 @@
         <f>0.01699</f>
         <v>1.6990000000000002E-2</v>
       </c>
+      <c r="S3">
+        <f>0.01232</f>
+        <v>1.2319999999999999E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>8</f>
         <v>8</v>
@@ -3273,6 +3356,10 @@
         <f>0.0009999</f>
         <v>9.9989999999999996E-4</v>
       </c>
+      <c r="D4">
+        <f>88/100000</f>
+        <v>8.8000000000000003E-4</v>
+      </c>
       <c r="J4">
         <f>8</f>
         <v>8</v>
@@ -3285,6 +3372,10 @@
         <f>0.00771</f>
         <v>7.7099999999999998E-3</v>
       </c>
+      <c r="M4">
+        <f>0.00576</f>
+        <v>5.7600000000000004E-3</v>
+      </c>
       <c r="P4">
         <f>12</f>
         <v>12</v>
@@ -3297,8 +3388,12 @@
         <f>0.00747</f>
         <v>7.4700000000000001E-3</v>
       </c>
+      <c r="S4">
+        <f>0.004618</f>
+        <v>4.6179999999999997E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>9</f>
         <v>9</v>
@@ -3311,6 +3406,9 @@
         <f>0.00019</f>
         <v>1.9000000000000001E-4</v>
       </c>
+      <c r="D5" s="1">
+        <v>1.6000000000000001E-4</v>
+      </c>
       <c r="J5">
         <f>9</f>
         <v>9</v>
@@ -3323,6 +3421,10 @@
         <f>0.0029</f>
         <v>2.8999999999999998E-3</v>
       </c>
+      <c r="M5">
+        <f>0.00196</f>
+        <v>1.9599999999999999E-3</v>
+      </c>
       <c r="P5">
         <f>13</f>
         <v>13</v>
@@ -3335,8 +3437,12 @@
         <f>0.00289</f>
         <v>2.8900000000000002E-3</v>
       </c>
+      <c r="S5">
+        <f>0.001342</f>
+        <v>1.3420000000000001E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>10</f>
         <v>10</v>
@@ -3349,6 +3455,10 @@
         <f>0.00004</f>
         <v>4.0000000000000003E-5</v>
       </c>
+      <c r="D6" s="1">
+        <f>0.000017</f>
+        <v>1.7E-5</v>
+      </c>
       <c r="J6">
         <f>10</f>
         <v>10</v>
@@ -3361,6 +3471,10 @@
         <f>0.00089</f>
         <v>8.8999999999999995E-4</v>
       </c>
+      <c r="M6">
+        <f>0.00049</f>
+        <v>4.8999999999999998E-4</v>
+      </c>
       <c r="P6">
         <f>14</f>
         <v>14</v>
@@ -3373,8 +3487,12 @@
         <f>0.00058</f>
         <v>5.8E-4</v>
       </c>
+      <c r="S6">
+        <f>0.000292</f>
+        <v>2.92E-4</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J7">
         <f>11</f>
         <v>11</v>
@@ -3387,6 +3505,10 @@
         <f>0.00009</f>
         <v>9.0000000000000006E-5</v>
       </c>
+      <c r="M7" s="1">
+        <f>0.000076</f>
+        <v>7.6000000000000004E-5</v>
+      </c>
       <c r="P7">
         <f>15</f>
         <v>15</v>
@@ -3399,8 +3521,12 @@
         <f>0.00021</f>
         <v>2.1000000000000001E-4</v>
       </c>
+      <c r="S7">
+        <f>0.000034</f>
+        <v>3.4E-5</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J8">
         <f>12</f>
         <v>12</v>
@@ -3413,6 +3539,10 @@
         <f>0.00002</f>
         <v>2.0000000000000002E-5</v>
       </c>
+      <c r="M8">
+        <f>0.000012</f>
+        <v>1.2E-5</v>
+      </c>
       <c r="P8">
         <f>16</f>
         <v>16</v>
@@ -3424,6 +3554,10 @@
       <c r="R8">
         <f>0.00003</f>
         <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="S8">
+        <f>0.000008</f>
+        <v>7.9999999999999996E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added another layer of modulo blocks that should improve BER in the simple Non-Coherent detection code N=3. Duplicated 'DPSK No USRP' to begin implementation of the Non-Coherent detector N=2.
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/728999eba1fe14f3/Desktop/Simulink Holding Folder/Simulink Upload/dpsk Non-Coher N=2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peytonaplin\Desktop\NASA-Simulink-Projects\Simulink Upload\dpsk Non-Coher N=2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{5A60CA98-A86E-473F-9745-E9D2856C0FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C30A33E1-7780-4347-A68A-DAF936191834}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AFF1B-04A3-4952-80C1-A66AC32467F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>SNR</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>P. N=2</t>
+  </si>
+  <si>
+    <t>DS N=2</t>
+  </si>
+  <si>
+    <t>DS N=3</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Div&amp;Simon</c:v>
+            <c:v>DS N=2</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -215,16 +221,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0000000000000001E-4</c:v>
+                  <c:v>3.0000000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0000000000000004E-5</c:v>
+                  <c:v>5.0000000000000002E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,10 +350,10 @@
                   <c:v>3.0699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8000000000000003E-4</c:v>
+                  <c:v>8.4599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>1.6000000000000001E-4</c:v>
+                  <c:v>1.4999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
                   <c:v>1.7E-5</c:v>
@@ -359,6 +365,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-7E8F-48B7-BFAC-365A656D806F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>DS N=3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0000000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-928E-4014-97C1-45060FE9BD01}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -894,19 +960,19 @@
                   <c:v>1.379E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.7600000000000004E-3</c:v>
+                  <c:v>5.5319999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9599999999999999E-3</c:v>
+                  <c:v>1.758E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8999999999999998E-4</c:v>
+                  <c:v>4.3800000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>7.6000000000000004E-5</c:v>
+                  <c:v>6.2000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2E-5</c:v>
+                  <c:v>7.9999999999999996E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1474,7 +1540,7 @@
                   <c:v>4.6179999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3420000000000001E-3</c:v>
+                  <c:v>1.34E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.92E-4</c:v>
@@ -1483,7 +1549,7 @@
                   <c:v>3.4E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9999999999999996E-6</c:v>
+                  <c:v>9.9999999999999995E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3239,12 +3305,12 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3255,12 +3321,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -3268,6 +3334,9 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
@@ -3293,14 +3362,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>7</f>
         <v>7</v>
       </c>
       <c r="B3">
-        <f>3*10^-3</f>
-        <v>3.0000000000000001E-3</v>
+        <f>5*10^-3</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C3">
         <f>0.0034</f>
@@ -3310,6 +3379,10 @@
         <f>0.00307</f>
         <v>3.0699999999999998E-3</v>
       </c>
+      <c r="E3">
+        <f>0.004</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="J3">
         <f>7</f>
         <v>7</v>
@@ -3343,7 +3416,7 @@
         <v>1.2319999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>8</f>
         <v>8</v>
@@ -3357,8 +3430,12 @@
         <v>9.9989999999999996E-4</v>
       </c>
       <c r="D4">
-        <f>88/100000</f>
-        <v>8.8000000000000003E-4</v>
+        <f>0.000846</f>
+        <v>8.4599999999999996E-4</v>
+      </c>
+      <c r="E4">
+        <f>0.0008</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="J4">
         <f>8</f>
@@ -3373,8 +3450,8 @@
         <v>7.7099999999999998E-3</v>
       </c>
       <c r="M4">
-        <f>0.00576</f>
-        <v>5.7600000000000004E-3</v>
+        <f>0.005532</f>
+        <v>5.5319999999999996E-3</v>
       </c>
       <c r="P4">
         <f>12</f>
@@ -3393,21 +3470,25 @@
         <v>4.6179999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>9</f>
         <v>9</v>
       </c>
       <c r="B5">
-        <f>2*10^-4</f>
-        <v>2.0000000000000001E-4</v>
+        <f>3*10^-4</f>
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="C5">
         <f>0.00019</f>
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="D5" s="1">
-        <v>1.6000000000000001E-4</v>
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="E5">
+        <f>0.0001</f>
+        <v>1E-4</v>
       </c>
       <c r="J5">
         <f>9</f>
@@ -3422,8 +3503,8 @@
         <v>2.8999999999999998E-3</v>
       </c>
       <c r="M5">
-        <f>0.00196</f>
-        <v>1.9599999999999999E-3</v>
+        <f>0.001758</f>
+        <v>1.758E-3</v>
       </c>
       <c r="P5">
         <f>13</f>
@@ -3438,18 +3519,18 @@
         <v>2.8900000000000002E-3</v>
       </c>
       <c r="S5">
-        <f>0.001342</f>
-        <v>1.3420000000000001E-3</v>
+        <f>0.00134</f>
+        <v>1.34E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="B6">
-        <f>3*10^-5</f>
-        <v>3.0000000000000004E-5</v>
+        <f>5*10^-5</f>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="C6">
         <f>0.00004</f>
@@ -3459,6 +3540,10 @@
         <f>0.000017</f>
         <v>1.7E-5</v>
       </c>
+      <c r="E6">
+        <f>0.00001</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="J6">
         <f>10</f>
         <v>10</v>
@@ -3472,8 +3557,8 @@
         <v>8.8999999999999995E-4</v>
       </c>
       <c r="M6">
-        <f>0.00049</f>
-        <v>4.8999999999999998E-4</v>
+        <f>0.000438</f>
+        <v>4.3800000000000002E-4</v>
       </c>
       <c r="P6">
         <f>14</f>
@@ -3492,7 +3577,7 @@
         <v>2.92E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J7">
         <f>11</f>
         <v>11</v>
@@ -3506,8 +3591,8 @@
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="M7" s="1">
-        <f>0.000076</f>
-        <v>7.6000000000000004E-5</v>
+        <f>0.000062</f>
+        <v>6.2000000000000003E-5</v>
       </c>
       <c r="P7">
         <f>15</f>
@@ -3526,7 +3611,7 @@
         <v>3.4E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J8">
         <f>12</f>
         <v>12</v>
@@ -3540,8 +3625,8 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="M8">
-        <f>0.000012</f>
-        <v>1.2E-5</v>
+        <f>0.000008</f>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="P8">
         <f>16</f>
@@ -3556,8 +3641,8 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="S8">
-        <f>0.000008</f>
-        <v>7.9999999999999996E-6</v>
+        <f>0.000001</f>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizing changes to N=2, and N=3
</commit_message>
<xml_diff>
--- a/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
+++ b/Simulink Upload/dpsk Non-Coher N=2/Divsalar and Simon Compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peytonaplin\Desktop\NASA-Simulink-Projects\Simulink Upload\dpsk Non-Coher N=2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AFF1B-04A3-4952-80C1-A66AC32467F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F3FE64-EFDE-4DBB-9333-47B8DF60F93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0433A681-D541-45EB-A66B-92B1257F092A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>